<commit_message>
Removing older JSON files and updating naming to meet standards
Changed the naming of the locations in the Excel to match the files from the UN.  Some tidying up of unneeded files.
</commit_message>
<xml_diff>
--- a/TX BoQ v3-Python.xlsx
+++ b/TX BoQ v3-Python.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnmeye\Desktop\RFQ - Round 1 - July 2020\RFQ technical documents\Transmission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnmeye\Documents\GitHub\Ethiopia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F6B985-4561-43E0-BB1D-8EE58558EBF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E88F025-F263-4D5A-9DF8-92A018C1A67D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="No 800MHz" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="201">
   <si>
     <t>Y0</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Row Labels</t>
   </si>
   <si>
-    <t>Beninshangul Gumuz</t>
-  </si>
-  <si>
     <t>Dire Dawa</t>
   </si>
   <si>
@@ -642,6 +639,12 @@
   </si>
   <si>
     <t>What SDN use cases are you considering for Ethiopia? The standard vodafone grouping?</t>
+  </si>
+  <si>
+    <t>Benishangul Gumz</t>
+  </si>
+  <si>
+    <t>SNNP</t>
   </si>
 </sst>
 </file>
@@ -652,7 +655,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -976,7 +979,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1070,6 +1073,25 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1091,15 +1113,6 @@
     <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="6" builtinId="3"/>
@@ -3417,14 +3430,14 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="47.42578125" customWidth="1"/>
     <col min="14" max="14" width="7.85546875" customWidth="1"/>
     <col min="15" max="15" width="39.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -3459,7 +3472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -3500,7 +3513,7 @@
         <v>13733</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -3554,7 +3567,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15">
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -3609,7 +3622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -3664,7 +3677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -3719,7 +3732,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -3774,7 +3787,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -3829,7 +3842,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -3884,7 +3897,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="B11" t="s">
         <v>26</v>
       </c>
@@ -3939,7 +3952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -3994,7 +4007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="B13" t="s">
         <v>30</v>
       </c>
@@ -4038,7 +4051,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -4093,7 +4106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -4148,7 +4161,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="B16" t="s">
         <v>36</v>
       </c>
@@ -4203,7 +4216,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15">
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -4247,7 +4260,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15">
       <c r="B18" t="s">
         <v>40</v>
       </c>
@@ -4291,7 +4304,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15">
       <c r="B19" t="s">
         <v>42</v>
       </c>
@@ -4332,7 +4345,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15">
       <c r="B20" t="s">
         <v>44</v>
       </c>
@@ -4373,7 +4386,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15">
       <c r="B21" t="s">
         <v>45</v>
       </c>
@@ -4442,14 +4455,14 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="47.42578125" customWidth="1"/>
     <col min="14" max="14" width="7.85546875" customWidth="1"/>
     <col min="15" max="15" width="39.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -4484,7 +4497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -4525,7 +4538,7 @@
         <v>10891</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -4579,7 +4592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15">
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -4634,7 +4647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -4689,7 +4702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -4744,7 +4757,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -4799,7 +4812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -4854,7 +4867,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -4909,7 +4922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="B11" t="s">
         <v>26</v>
       </c>
@@ -4964,7 +4977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -5019,7 +5032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="B13" t="s">
         <v>46</v>
       </c>
@@ -5063,7 +5076,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -5118,7 +5131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -5173,7 +5186,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="B16" t="s">
         <v>36</v>
       </c>
@@ -5228,7 +5241,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15">
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -5272,7 +5285,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15">
       <c r="B18" t="s">
         <v>40</v>
       </c>
@@ -5316,7 +5329,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15">
       <c r="B19" t="s">
         <v>42</v>
       </c>
@@ -5357,7 +5370,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15">
       <c r="B20" t="s">
         <v>44</v>
       </c>
@@ -5415,12 +5428,12 @@
       <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="6" t="s">
         <v>47</v>
       </c>
@@ -5458,8 +5471,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:14">
+      <c r="A3" s="41" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="5">
@@ -5497,8 +5510,8 @@
       </c>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" s="42" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="3">
@@ -5535,8 +5548,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:14">
+      <c r="A5" s="43" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="3">
@@ -5573,8 +5586,8 @@
         <v>0.97802197802197799</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+    <row r="6" spans="1:14">
+      <c r="A6" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="3">
@@ -5611,8 +5624,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:14">
+      <c r="A7" s="44" t="s">
         <v>52</v>
       </c>
       <c r="B7" s="3">
@@ -5649,7 +5662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="6" t="s">
         <v>53</v>
       </c>
@@ -5687,7 +5700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
@@ -5725,7 +5738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="8" t="s">
         <v>55</v>
       </c>
@@ -5763,7 +5776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="8" t="s">
         <v>56</v>
       </c>
@@ -5801,7 +5814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="8" t="s">
         <v>57</v>
       </c>
@@ -5839,7 +5852,7 @@
         <v>0.6785714285714286</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
@@ -5877,7 +5890,7 @@
         <v>0.32142857142857145</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="11" t="s">
         <v>59</v>
       </c>
@@ -5915,7 +5928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -5953,7 +5966,7 @@
         <v>3.663003663003663E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -5991,7 +6004,7 @@
         <v>4.304029304029304E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -6029,7 +6042,7 @@
         <v>0.24358974358974358</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -6067,7 +6080,7 @@
         <v>1.9230769230769232E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -6105,7 +6118,7 @@
         <v>3.663003663003663E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -6143,7 +6156,7 @@
         <v>9.1575091575091579E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -6181,7 +6194,7 @@
         <v>8.241758241758242E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -6219,7 +6232,7 @@
         <v>0.45421245421245421</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -6257,7 +6270,7 @@
         <v>7.5091575091575088E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -6295,7 +6308,7 @@
         <v>9.5238095238095233E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -6350,33 +6363,33 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.5703125" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="15.6" customHeight="1">
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="60"/>
       <c r="O3" s="24"/>
     </row>
-    <row r="4" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
+    <row r="4" spans="2:15" ht="15.75">
+      <c r="B4" s="61"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="16" t="s">
         <v>72</v>
       </c>
@@ -6414,7 +6427,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15">
       <c r="B5" s="17" t="s">
         <v>83</v>
       </c>
@@ -6467,7 +6480,7 @@
       </c>
       <c r="O5" s="22"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15">
       <c r="B6" s="17" t="s">
         <v>85</v>
       </c>
@@ -6520,7 +6533,7 @@
       </c>
       <c r="O6" s="22"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="B7" s="17" t="s">
         <v>85</v>
       </c>
@@ -6573,7 +6586,7 @@
       </c>
       <c r="O7" s="22"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="B8" s="17" t="s">
         <v>85</v>
       </c>
@@ -6626,7 +6639,7 @@
       </c>
       <c r="O8" s="22"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="B9" s="17" t="s">
         <v>85</v>
       </c>
@@ -6679,7 +6692,7 @@
       </c>
       <c r="O9" s="22"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="B10" s="20"/>
       <c r="C10" s="21"/>
       <c r="D10" s="28">
@@ -6728,26 +6741,26 @@
       </c>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" ht="15.75">
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="43"/>
-    </row>
-    <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="60"/>
+    </row>
+    <row r="12" spans="2:15" ht="15.75">
+      <c r="B12" s="61"/>
+      <c r="C12" s="62"/>
       <c r="D12" s="16" t="s">
         <v>72</v>
       </c>
@@ -6782,7 +6795,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="B13" s="17" t="s">
         <v>83</v>
       </c>
@@ -6834,7 +6847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="B14" s="17" t="s">
         <v>85</v>
       </c>
@@ -6886,7 +6899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="B15" s="17" t="s">
         <v>85</v>
       </c>
@@ -6938,7 +6951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="B16" s="17" t="s">
         <v>85</v>
       </c>
@@ -6990,7 +7003,7 @@
         <v>49.241169544740977</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14">
       <c r="B17" s="17" t="s">
         <v>85</v>
       </c>
@@ -7042,7 +7055,7 @@
         <v>23.324764521193092</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14">
       <c r="D18" s="28">
         <f>SUM(D13:D17)</f>
         <v>59.957470010905126</v>
@@ -7088,24 +7101,24 @@
         <v>72.565934065934073</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="46" t="s">
+    <row r="19" spans="2:14">
+      <c r="D19" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-    </row>
-    <row r="20" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+    </row>
+    <row r="20" spans="2:14" ht="15.75">
+      <c r="B20" s="61"/>
+      <c r="C20" s="62"/>
       <c r="D20" s="16" t="s">
         <v>72</v>
       </c>
@@ -7140,7 +7153,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14">
       <c r="B21" s="17" t="s">
         <v>83</v>
       </c>
@@ -7192,7 +7205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14">
       <c r="B22" s="17" t="s">
         <v>85</v>
       </c>
@@ -7244,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14">
       <c r="B23" s="17" t="s">
         <v>85</v>
       </c>
@@ -7296,7 +7309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14">
       <c r="B24" s="17" t="s">
         <v>85</v>
       </c>
@@ -7348,7 +7361,7 @@
         <v>278.68406593406593</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14">
       <c r="B25" s="17" t="s">
         <v>85</v>
       </c>
@@ -7400,7 +7413,7 @@
         <v>132.00824175824175</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14">
       <c r="D26" s="28">
         <f>SUM(D21:D25)</f>
         <v>364.13195201744821</v>
@@ -7446,24 +7459,24 @@
         <v>410.69230769230768</v>
       </c>
     </row>
-    <row r="27" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="46" t="s">
+    <row r="27" spans="2:14" ht="14.45" customHeight="1">
+      <c r="D27" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-    </row>
-    <row r="28" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="44"/>
-      <c r="C28" s="45"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+    </row>
+    <row r="28" spans="2:14" ht="15.75">
+      <c r="B28" s="61"/>
+      <c r="C28" s="62"/>
       <c r="D28" s="16" t="s">
         <v>72</v>
       </c>
@@ -7498,7 +7511,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14">
       <c r="B29" s="17" t="s">
         <v>83</v>
       </c>
@@ -7550,7 +7563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14">
       <c r="B30" s="17" t="s">
         <v>85</v>
       </c>
@@ -7602,7 +7615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14">
       <c r="B31" s="17" t="s">
         <v>85</v>
       </c>
@@ -7654,7 +7667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14">
       <c r="B32" s="17" t="s">
         <v>85</v>
       </c>
@@ -7706,7 +7719,7 @@
         <v>22.001373626373628</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14">
       <c r="B33" s="17" t="s">
         <v>85</v>
       </c>
@@ -7758,7 +7771,7 @@
         <v>10.421703296703297</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14">
       <c r="D34" s="28">
         <f>SUM(D29:D33)</f>
         <v>27.785169029443836</v>
@@ -7804,24 +7817,24 @@
         <v>32.423076923076927</v>
       </c>
     </row>
-    <row r="35" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="46" t="s">
+    <row r="35" spans="2:14" ht="14.45" customHeight="1">
+      <c r="D35" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
-    </row>
-    <row r="36" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="44"/>
-      <c r="C36" s="45"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="64"/>
+    </row>
+    <row r="36" spans="2:14" ht="15.75">
+      <c r="B36" s="61"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="16" t="s">
         <v>72</v>
       </c>
@@ -7856,7 +7869,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14">
       <c r="B37" s="17" t="s">
         <v>83</v>
       </c>
@@ -7908,7 +7921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14">
       <c r="B38" s="17" t="s">
         <v>85</v>
       </c>
@@ -7960,7 +7973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14">
       <c r="B39" s="17" t="s">
         <v>85</v>
       </c>
@@ -8012,7 +8025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14">
       <c r="B40" s="17" t="s">
         <v>85</v>
       </c>
@@ -8064,7 +8077,7 @@
         <v>4.1907378335949765</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14">
       <c r="B41" s="17" t="s">
         <v>85</v>
       </c>
@@ -8116,7 +8129,7 @@
         <v>1.9850863422291996</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14">
       <c r="D42" s="28">
         <f>SUM(D37:D41)</f>
         <v>43.871319520174481</v>
@@ -8162,24 +8175,24 @@
         <v>6.1758241758241761</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D43" s="46" t="s">
+    <row r="43" spans="2:14">
+      <c r="D43" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="47"/>
-      <c r="M43" s="47"/>
-      <c r="N43" s="47"/>
-    </row>
-    <row r="44" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="44"/>
-      <c r="C44" s="45"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="64"/>
+      <c r="K43" s="64"/>
+      <c r="L43" s="64"/>
+      <c r="M43" s="64"/>
+      <c r="N43" s="64"/>
+    </row>
+    <row r="44" spans="2:14" ht="15.75">
+      <c r="B44" s="61"/>
+      <c r="C44" s="62"/>
       <c r="D44" s="16" t="s">
         <v>72</v>
       </c>
@@ -8214,7 +8227,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14">
       <c r="B45" s="17" t="s">
         <v>83</v>
       </c>
@@ -8266,7 +8279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14">
       <c r="B46" s="17" t="s">
         <v>85</v>
       </c>
@@ -8318,7 +8331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14">
       <c r="B47" s="17" t="s">
         <v>85</v>
       </c>
@@ -8370,7 +8383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14">
       <c r="B48" s="17" t="s">
         <v>85</v>
       </c>
@@ -8422,7 +8435,7 @@
         <v>10.476844583987441</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14">
       <c r="B49" s="17" t="s">
         <v>85</v>
       </c>
@@ -8474,7 +8487,7 @@
         <v>4.9627158555729984</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14">
       <c r="D50" s="28">
         <f>SUM(D45:D49)</f>
         <v>14.623773173391495</v>
@@ -8520,24 +8533,24 @@
         <v>15.43956043956044</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D51" s="46" t="s">
+    <row r="51" spans="2:14">
+      <c r="D51" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="47"/>
-      <c r="L51" s="47"/>
-      <c r="M51" s="47"/>
-      <c r="N51" s="47"/>
-    </row>
-    <row r="52" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="44"/>
-      <c r="C52" s="45"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
+      <c r="H51" s="64"/>
+      <c r="I51" s="64"/>
+      <c r="J51" s="64"/>
+      <c r="K51" s="64"/>
+      <c r="L51" s="64"/>
+      <c r="M51" s="64"/>
+      <c r="N51" s="64"/>
+    </row>
+    <row r="52" spans="2:14" ht="15.75">
+      <c r="B52" s="61"/>
+      <c r="C52" s="62"/>
       <c r="D52" s="16" t="s">
         <v>72</v>
       </c>
@@ -8572,7 +8585,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14">
       <c r="B53" s="17" t="s">
         <v>83</v>
       </c>
@@ -8624,7 +8637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14">
       <c r="B54" s="17" t="s">
         <v>85</v>
       </c>
@@ -8676,7 +8689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14">
       <c r="B55" s="17" t="s">
         <v>85</v>
       </c>
@@ -8728,7 +8741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14">
       <c r="B56" s="17" t="s">
         <v>85</v>
       </c>
@@ -8780,7 +8793,7 @@
         <v>9.4291601255886981</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14">
       <c r="B57" s="17" t="s">
         <v>85</v>
       </c>
@@ -8832,7 +8845,7 @@
         <v>4.4664442700156997</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14">
       <c r="D58" s="28">
         <f>SUM(D53:D57)</f>
         <v>32.172300981461291</v>
@@ -8878,24 +8891,24 @@
         <v>13.895604395604398</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D59" s="46" t="s">
+    <row r="59" spans="2:14">
+      <c r="D59" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="47"/>
-      <c r="I59" s="47"/>
-      <c r="J59" s="47"/>
-      <c r="K59" s="47"/>
-      <c r="L59" s="47"/>
-      <c r="M59" s="47"/>
-      <c r="N59" s="47"/>
-    </row>
-    <row r="60" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="44"/>
-      <c r="C60" s="45"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="64"/>
+      <c r="H59" s="64"/>
+      <c r="I59" s="64"/>
+      <c r="J59" s="64"/>
+      <c r="K59" s="64"/>
+      <c r="L59" s="64"/>
+      <c r="M59" s="64"/>
+      <c r="N59" s="64"/>
+    </row>
+    <row r="60" spans="2:14" ht="15.75">
+      <c r="B60" s="61"/>
+      <c r="C60" s="62"/>
       <c r="D60" s="16" t="s">
         <v>72</v>
       </c>
@@ -8930,7 +8943,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14">
       <c r="B61" s="17" t="s">
         <v>83</v>
       </c>
@@ -8982,7 +8995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14">
       <c r="B62" s="17" t="s">
         <v>85</v>
       </c>
@@ -9034,7 +9047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14">
       <c r="B63" s="17" t="s">
         <v>85</v>
       </c>
@@ -9086,7 +9099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14">
       <c r="B64" s="17" t="s">
         <v>85</v>
       </c>
@@ -9138,7 +9151,7 @@
         <v>519.65149136577713</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14">
       <c r="B65" s="17" t="s">
         <v>85</v>
       </c>
@@ -9190,7 +9203,7 @@
         <v>246.15070643642073</v>
       </c>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14">
       <c r="D66" s="28">
         <f>SUM(D61:D65)</f>
         <v>231.0556161395856</v>
@@ -9236,24 +9249,24 @@
         <v>765.80219780219784</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D67" s="46" t="s">
+    <row r="67" spans="2:14">
+      <c r="D67" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
-      <c r="H67" s="47"/>
-      <c r="I67" s="47"/>
-      <c r="J67" s="47"/>
-      <c r="K67" s="47"/>
-      <c r="L67" s="47"/>
-      <c r="M67" s="47"/>
-      <c r="N67" s="47"/>
-    </row>
-    <row r="68" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="44"/>
-      <c r="C68" s="45"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="64"/>
+      <c r="I67" s="64"/>
+      <c r="J67" s="64"/>
+      <c r="K67" s="64"/>
+      <c r="L67" s="64"/>
+      <c r="M67" s="64"/>
+      <c r="N67" s="64"/>
+    </row>
+    <row r="68" spans="2:14" ht="15.75">
+      <c r="B68" s="61"/>
+      <c r="C68" s="62"/>
       <c r="D68" s="16" t="s">
         <v>72</v>
       </c>
@@ -9288,7 +9301,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14">
       <c r="B69" s="17" t="s">
         <v>83</v>
       </c>
@@ -9340,7 +9353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:14">
       <c r="B70" s="17" t="s">
         <v>85</v>
       </c>
@@ -9392,7 +9405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:14">
       <c r="B71" s="17" t="s">
         <v>85</v>
       </c>
@@ -9444,7 +9457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:14">
       <c r="B72" s="17" t="s">
         <v>85</v>
       </c>
@@ -9496,7 +9509,7 @@
         <v>85.910125588697014</v>
       </c>
     </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:14">
       <c r="B73" s="17" t="s">
         <v>85</v>
       </c>
@@ -9548,24 +9561,24 @@
         <v>40.694270015698592</v>
       </c>
     </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D75" s="46" t="s">
+    <row r="75" spans="2:14">
+      <c r="D75" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="E75" s="47"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="47"/>
-      <c r="H75" s="47"/>
-      <c r="I75" s="47"/>
-      <c r="J75" s="47"/>
-      <c r="K75" s="47"/>
-      <c r="L75" s="47"/>
-      <c r="M75" s="47"/>
-      <c r="N75" s="47"/>
-    </row>
-    <row r="76" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B76" s="44"/>
-      <c r="C76" s="45"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="64"/>
+      <c r="H75" s="64"/>
+      <c r="I75" s="64"/>
+      <c r="J75" s="64"/>
+      <c r="K75" s="64"/>
+      <c r="L75" s="64"/>
+      <c r="M75" s="64"/>
+      <c r="N75" s="64"/>
+    </row>
+    <row r="76" spans="2:14" ht="15.75">
+      <c r="B76" s="61"/>
+      <c r="C76" s="62"/>
       <c r="D76" s="16" t="s">
         <v>72</v>
       </c>
@@ -9600,7 +9613,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:14">
       <c r="B77" s="17" t="s">
         <v>83</v>
       </c>
@@ -9652,7 +9665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:14">
       <c r="B78" s="17" t="s">
         <v>85</v>
       </c>
@@ -9704,7 +9717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:14">
       <c r="B79" s="17" t="s">
         <v>85</v>
       </c>
@@ -9756,7 +9769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14">
       <c r="B80" s="17" t="s">
         <v>85</v>
       </c>
@@ -9808,7 +9821,7 @@
         <v>108.9591836734694</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:14">
       <c r="B81" s="17" t="s">
         <v>85</v>
       </c>
@@ -9860,24 +9873,24 @@
         <v>51.612244897959179</v>
       </c>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D83" s="46" t="s">
+    <row r="83" spans="2:14">
+      <c r="D83" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="E83" s="47"/>
-      <c r="F83" s="47"/>
-      <c r="G83" s="47"/>
-      <c r="H83" s="47"/>
-      <c r="I83" s="47"/>
-      <c r="J83" s="47"/>
-      <c r="K83" s="47"/>
-      <c r="L83" s="47"/>
-      <c r="M83" s="47"/>
-      <c r="N83" s="47"/>
-    </row>
-    <row r="84" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B84" s="44"/>
-      <c r="C84" s="45"/>
+      <c r="E83" s="64"/>
+      <c r="F83" s="64"/>
+      <c r="G83" s="64"/>
+      <c r="H83" s="64"/>
+      <c r="I83" s="64"/>
+      <c r="J83" s="64"/>
+      <c r="K83" s="64"/>
+      <c r="L83" s="64"/>
+      <c r="M83" s="64"/>
+      <c r="N83" s="64"/>
+    </row>
+    <row r="84" spans="2:14" ht="15.75">
+      <c r="B84" s="61"/>
+      <c r="C84" s="62"/>
       <c r="D84" s="16" t="s">
         <v>72</v>
       </c>
@@ -9912,7 +9925,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:14">
       <c r="B85" s="17" t="s">
         <v>83</v>
       </c>
@@ -9964,7 +9977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:14">
       <c r="B86" s="17" t="s">
         <v>85</v>
       </c>
@@ -10016,7 +10029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:14">
       <c r="B87" s="17" t="s">
         <v>85</v>
       </c>
@@ -10068,7 +10081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:14">
       <c r="B88" s="17" t="s">
         <v>85</v>
       </c>
@@ -10120,7 +10133,7 @@
         <v>51.336538461538467</v>
       </c>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14">
       <c r="B89" s="17" t="s">
         <v>85</v>
       </c>
@@ -10172,24 +10185,24 @@
         <v>24.317307692307693</v>
       </c>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D91" s="46" t="s">
+    <row r="91" spans="2:14">
+      <c r="D91" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="E91" s="47"/>
-      <c r="F91" s="47"/>
-      <c r="G91" s="47"/>
-      <c r="H91" s="47"/>
-      <c r="I91" s="47"/>
-      <c r="J91" s="47"/>
-      <c r="K91" s="47"/>
-      <c r="L91" s="47"/>
-      <c r="M91" s="47"/>
-      <c r="N91" s="47"/>
-    </row>
-    <row r="92" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B92" s="44"/>
-      <c r="C92" s="45"/>
+      <c r="E91" s="64"/>
+      <c r="F91" s="64"/>
+      <c r="G91" s="64"/>
+      <c r="H91" s="64"/>
+      <c r="I91" s="64"/>
+      <c r="J91" s="64"/>
+      <c r="K91" s="64"/>
+      <c r="L91" s="64"/>
+      <c r="M91" s="64"/>
+      <c r="N91" s="64"/>
+    </row>
+    <row r="92" spans="2:14" ht="15.75">
+      <c r="B92" s="61"/>
+      <c r="C92" s="62"/>
       <c r="D92" s="16" t="s">
         <v>72</v>
       </c>
@@ -10224,7 +10237,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:14">
       <c r="B93" s="17" t="s">
         <v>83</v>
       </c>
@@ -10276,7 +10289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:14">
       <c r="B94" s="17" t="s">
         <v>85</v>
       </c>
@@ -10328,7 +10341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:14">
       <c r="B95" s="17" t="s">
         <v>85</v>
       </c>
@@ -10380,7 +10393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:14">
       <c r="B96" s="17" t="s">
         <v>85</v>
       </c>
@@ -10432,7 +10445,7 @@
         <v>1144.0714285714289</v>
       </c>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:14">
       <c r="B97" s="17" t="s">
         <v>85</v>
       </c>
@@ -10523,21 +10536,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E399C830-DD96-4A5E-B3BC-68E8ADB24F95}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="12" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75">
       <c r="A1" s="26" t="s">
         <v>94</v>
       </c>
@@ -10548,43 +10561,43 @@
         <v>92</v>
       </c>
       <c r="D1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="I1" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="J1" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="K1" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="M1" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="N1" s="29" t="s">
         <v>122</v>
-      </c>
-      <c r="N1" s="29" t="s">
-        <v>123</v>
       </c>
       <c r="O1" s="33" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="17" t="s">
         <v>83</v>
       </c>
@@ -10632,7 +10645,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="17" t="s">
         <v>85</v>
       </c>
@@ -10680,7 +10693,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="17" t="s">
         <v>85</v>
       </c>
@@ -10728,7 +10741,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="17" t="s">
         <v>85</v>
       </c>
@@ -10776,7 +10789,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="17" t="s">
         <v>85</v>
       </c>
@@ -10824,7 +10837,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="17" t="s">
         <v>83</v>
       </c>
@@ -10872,7 +10885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="17" t="s">
         <v>85</v>
       </c>
@@ -10920,7 +10933,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="17" t="s">
         <v>85</v>
       </c>
@@ -10968,7 +10981,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="17" t="s">
         <v>85</v>
       </c>
@@ -11016,7 +11029,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="25" customFormat="1">
       <c r="A11" s="17" t="s">
         <v>85</v>
       </c>
@@ -11064,7 +11077,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="25" customFormat="1">
       <c r="A12" s="17" t="s">
         <v>83</v>
       </c>
@@ -11112,7 +11125,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="25" customFormat="1">
       <c r="A13" s="17" t="s">
         <v>85</v>
       </c>
@@ -11160,7 +11173,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" s="25" customFormat="1">
       <c r="A14" s="17" t="s">
         <v>85</v>
       </c>
@@ -11208,7 +11221,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="25" customFormat="1">
       <c r="A15" s="17" t="s">
         <v>85</v>
       </c>
@@ -11256,7 +11269,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="25" customFormat="1">
       <c r="A16" s="17" t="s">
         <v>85</v>
       </c>
@@ -11304,15 +11317,15 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="25" customFormat="1">
       <c r="A17" s="17" t="s">
         <v>83</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>98</v>
+      <c r="C17" s="48" t="s">
+        <v>199</v>
       </c>
       <c r="D17" s="22">
         <v>3</v>
@@ -11352,15 +11365,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="25" customFormat="1">
       <c r="A18" s="17" t="s">
         <v>85</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>98</v>
+      <c r="C18" s="49" t="s">
+        <v>199</v>
       </c>
       <c r="D18" s="22">
         <v>8</v>
@@ -11400,15 +11413,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="25" customFormat="1">
       <c r="A19" s="17" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>98</v>
+      <c r="C19" s="50" t="s">
+        <v>199</v>
       </c>
       <c r="D19" s="22">
         <v>3</v>
@@ -11448,15 +11461,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="25" customFormat="1">
       <c r="A20" s="17" t="s">
         <v>85</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>98</v>
+      <c r="C20" s="51" t="s">
+        <v>199</v>
       </c>
       <c r="D20" s="22">
         <v>5</v>
@@ -11496,15 +11509,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="25" customFormat="1">
       <c r="A21" s="17" t="s">
         <v>85</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>98</v>
+      <c r="C21" s="52" t="s">
+        <v>199</v>
       </c>
       <c r="D21" s="22">
         <v>9</v>
@@ -11544,7 +11557,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="25" customFormat="1">
       <c r="A22" s="17" t="s">
         <v>83</v>
       </c>
@@ -11552,7 +11565,7 @@
         <v>84</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="22">
         <v>4</v>
@@ -11592,7 +11605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="25" customFormat="1">
       <c r="A23" s="17" t="s">
         <v>85</v>
       </c>
@@ -11600,7 +11613,7 @@
         <v>55</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D23" s="22">
         <v>12</v>
@@ -11640,7 +11653,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="25" customFormat="1">
       <c r="A24" s="17" t="s">
         <v>85</v>
       </c>
@@ -11648,7 +11661,7 @@
         <v>56</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" s="22">
         <v>6</v>
@@ -11688,7 +11701,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="25" customFormat="1">
       <c r="A25" s="17" t="s">
         <v>85</v>
       </c>
@@ -11696,7 +11709,7 @@
         <v>57</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="22">
         <v>8</v>
@@ -11736,7 +11749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="25" customFormat="1">
       <c r="A26" s="17" t="s">
         <v>85</v>
       </c>
@@ -11744,7 +11757,7 @@
         <v>58</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D26" s="22">
         <v>14</v>
@@ -11784,7 +11797,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="25" customFormat="1">
       <c r="A27" s="17" t="s">
         <v>83</v>
       </c>
@@ -11832,7 +11845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="25" customFormat="1">
       <c r="A28" s="17" t="s">
         <v>85</v>
       </c>
@@ -11880,7 +11893,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="25" customFormat="1">
       <c r="A29" s="17" t="s">
         <v>85</v>
       </c>
@@ -11928,7 +11941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="25" customFormat="1">
       <c r="A30" s="17" t="s">
         <v>85</v>
       </c>
@@ -11976,7 +11989,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="25" customFormat="1">
       <c r="A31" s="17" t="s">
         <v>85</v>
       </c>
@@ -12024,7 +12037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="25" customFormat="1">
       <c r="A32" s="17" t="s">
         <v>83</v>
       </c>
@@ -12072,7 +12085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="25" customFormat="1">
       <c r="A33" s="17" t="s">
         <v>85</v>
       </c>
@@ -12120,7 +12133,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="25" customFormat="1">
       <c r="A34" s="17" t="s">
         <v>85</v>
       </c>
@@ -12168,7 +12181,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="25" customFormat="1">
       <c r="A35" s="17" t="s">
         <v>85</v>
       </c>
@@ -12216,7 +12229,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="25" customFormat="1">
       <c r="A36" s="17" t="s">
         <v>85</v>
       </c>
@@ -12264,7 +12277,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="25" customFormat="1">
       <c r="A37" s="17" t="s">
         <v>83</v>
       </c>
@@ -12312,7 +12325,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="25" customFormat="1">
       <c r="A38" s="17" t="s">
         <v>85</v>
       </c>
@@ -12360,7 +12373,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="25" customFormat="1">
       <c r="A39" s="17" t="s">
         <v>85</v>
       </c>
@@ -12408,7 +12421,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="25" customFormat="1">
       <c r="A40" s="17" t="s">
         <v>85</v>
       </c>
@@ -12456,7 +12469,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="25" customFormat="1">
       <c r="A41" s="17" t="s">
         <v>85</v>
       </c>
@@ -12504,15 +12517,15 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="25" customFormat="1">
       <c r="A42" s="17" t="s">
         <v>83</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="18" t="s">
-        <v>68</v>
+      <c r="C42" s="53" t="s">
+        <v>200</v>
       </c>
       <c r="D42" s="22">
         <v>6</v>
@@ -12552,15 +12565,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="25" customFormat="1">
       <c r="A43" s="17" t="s">
         <v>85</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="18" t="s">
-        <v>68</v>
+      <c r="C43" s="55" t="s">
+        <v>200</v>
       </c>
       <c r="D43" s="22">
         <v>19</v>
@@ -12600,15 +12613,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="25" customFormat="1">
       <c r="A44" s="17" t="s">
         <v>85</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="18" t="s">
-        <v>68</v>
+      <c r="C44" s="54" t="s">
+        <v>200</v>
       </c>
       <c r="D44" s="22">
         <v>8</v>
@@ -12648,15 +12661,15 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="25" customFormat="1">
       <c r="A45" s="17" t="s">
         <v>85</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="18" t="s">
-        <v>68</v>
+      <c r="C45" s="56" t="s">
+        <v>200</v>
       </c>
       <c r="D45" s="22">
         <v>13</v>
@@ -12696,15 +12709,15 @@
         <v>750</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="25" customFormat="1">
       <c r="A46" s="17" t="s">
         <v>85</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="18" t="s">
-        <v>68</v>
+      <c r="C46" s="57" t="s">
+        <v>200</v>
       </c>
       <c r="D46" s="22">
         <v>22</v>
@@ -12744,7 +12757,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="47" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="25" customFormat="1">
       <c r="A47" s="17" t="s">
         <v>83</v>
       </c>
@@ -12752,7 +12765,7 @@
         <v>84</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D47" s="22">
         <v>15</v>
@@ -12792,7 +12805,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="25" customFormat="1">
       <c r="A48" s="17" t="s">
         <v>85</v>
       </c>
@@ -12800,7 +12813,7 @@
         <v>55</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D48" s="22">
         <v>46</v>
@@ -12840,7 +12853,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" s="25" customFormat="1">
       <c r="A49" s="17" t="s">
         <v>85</v>
       </c>
@@ -12848,7 +12861,7 @@
         <v>56</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D49" s="22">
         <v>19</v>
@@ -12888,7 +12901,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="25" customFormat="1">
       <c r="A50" s="17" t="s">
         <v>85</v>
       </c>
@@ -12896,7 +12909,7 @@
         <v>57</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D50" s="22">
         <v>31</v>
@@ -12936,7 +12949,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="25" customFormat="1">
       <c r="A51" s="17" t="s">
         <v>85</v>
       </c>
@@ -12944,7 +12957,7 @@
         <v>58</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D51" s="22">
         <v>52</v>
@@ -12984,7 +12997,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="25" customFormat="1">
       <c r="A52" s="17" t="s">
         <v>83</v>
       </c>
@@ -12992,7 +13005,7 @@
         <v>84</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D52" s="22">
         <v>5</v>
@@ -13032,7 +13045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" s="25" customFormat="1">
       <c r="A53" s="17" t="s">
         <v>85</v>
       </c>
@@ -13040,7 +13053,7 @@
         <v>55</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" s="22">
         <v>15</v>
@@ -13080,7 +13093,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" s="25" customFormat="1">
       <c r="A54" s="17" t="s">
         <v>85</v>
       </c>
@@ -13088,7 +13101,7 @@
         <v>56</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" s="22">
         <v>6</v>
@@ -13128,7 +13141,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" s="25" customFormat="1">
       <c r="A55" s="17" t="s">
         <v>85</v>
       </c>
@@ -13136,7 +13149,7 @@
         <v>57</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D55" s="22">
         <v>10</v>
@@ -13176,7 +13189,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" s="25" customFormat="1">
       <c r="A56" s="17" t="s">
         <v>85</v>
       </c>
@@ -13184,7 +13197,7 @@
         <v>58</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D56" s="22">
         <v>17</v>
@@ -13242,52 +13255,52 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="31" t="s">
         <v>97</v>
       </c>
       <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
         <v>102</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>103</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>104</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>105</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>106</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>107</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>108</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>109</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>110</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>111</v>
       </c>
-      <c r="L3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="32" t="s">
         <v>71</v>
       </c>
@@ -13325,7 +13338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="32" t="s">
         <v>86</v>
       </c>
@@ -13363,7 +13376,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="32" t="s">
         <v>87</v>
       </c>
@@ -13401,7 +13414,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="32" t="s">
         <v>63</v>
       </c>
@@ -13439,7 +13452,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="32" t="s">
         <v>64</v>
       </c>
@@ -13477,7 +13490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="32" t="s">
         <v>89</v>
       </c>
@@ -13515,7 +13528,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="32" t="s">
         <v>90</v>
       </c>
@@ -13553,7 +13566,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="32" t="s">
         <v>68</v>
       </c>
@@ -13591,7 +13604,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="32" t="s">
         <v>69</v>
       </c>
@@ -13629,7 +13642,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="32" t="s">
         <v>70</v>
       </c>
@@ -13667,7 +13680,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="32" t="s">
         <v>95</v>
       </c>
@@ -13705,7 +13718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="32" t="s">
         <v>96</v>
       </c>
@@ -13752,80 +13765,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7EFFE79-863F-4267-9C99-730664104053}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="A45" sqref="A45:D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
         <v>125</v>
       </c>
-      <c r="C2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
         <v>127</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1">
+      <c r="C4" s="34" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="34" t="s">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C5" s="35" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="35" t="s">
+      <c r="D5" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="E5" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="F5" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="37" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="26.25" thickBot="1">
+      <c r="C6" s="38" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="39" t="s">
         <v>134</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>135</v>
       </c>
       <c r="E6" s="39">
         <v>620</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="64.5" thickBot="1">
       <c r="C7" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>86</v>
@@ -13834,102 +13847,102 @@
         <v>571</v>
       </c>
       <c r="F7" s="40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="39" thickBot="1">
+      <c r="C8" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="39" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>138</v>
       </c>
       <c r="E8" s="39">
         <v>323</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26.25" thickBot="1">
       <c r="C9" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" s="39">
         <v>949</v>
       </c>
       <c r="F9" s="40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="90" thickBot="1">
+      <c r="C10" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="39" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="90" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>141</v>
       </c>
       <c r="E10" s="39">
         <v>1173</v>
       </c>
       <c r="F10" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="51.75" thickBot="1">
+      <c r="C11" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="39" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>143</v>
       </c>
       <c r="E11" s="39">
         <v>352</v>
       </c>
       <c r="F11" s="40" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1">
       <c r="C12" s="38" t="s">
         <v>86</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E12" s="39">
         <v>818</v>
       </c>
       <c r="F12" s="40"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1">
       <c r="C13" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E13" s="39">
         <v>383</v>
       </c>
       <c r="F13" s="40"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1">
       <c r="C14" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E14" s="39">
         <v>370</v>
       </c>
       <c r="F14" s="40"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
       <c r="C15" s="38" t="s">
         <v>91</v>
       </c>
@@ -13939,449 +13952,449 @@
       </c>
       <c r="F15" s="40"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.75">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>4</v>
       </c>
       <c r="B41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" t="s">
         <v>150</v>
       </c>
-      <c r="C41" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>5</v>
       </c>
       <c r="B42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" t="s">
         <v>147</v>
       </c>
-      <c r="C42" t="s">
+    </row>
+    <row r="43" spans="1:3">
+      <c r="C43" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="102" x14ac:dyDescent="0.25">
-      <c r="A45" s="52" t="s">
+    <row r="45" spans="1:3" ht="89.25">
+      <c r="A45" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" t="s">
         <v>152</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="C45" s="53" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="76.5">
+      <c r="A46" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C46" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="C46" s="53" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="76.5">
+      <c r="A47" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" s="46" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B47" t="s">
-        <v>155</v>
-      </c>
-      <c r="C47" s="53" t="s">
+    <row r="48" spans="1:3" ht="51">
+      <c r="A48" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="46" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="51" x14ac:dyDescent="0.25">
-      <c r="A48" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B48" t="s">
-        <v>155</v>
-      </c>
-      <c r="C48" s="53" t="s">
+    <row r="49" spans="1:3" ht="38.25">
+      <c r="A49" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" s="46" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B49" t="s">
-        <v>155</v>
-      </c>
-      <c r="C49" s="53" t="s">
+    <row r="50" spans="1:3" ht="25.5">
+      <c r="A50" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" s="46" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B50" t="s">
-        <v>155</v>
-      </c>
-      <c r="C50" s="53" t="s">
+    <row r="51" spans="1:3" ht="63.75">
+      <c r="A51" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" s="46" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B51" t="s">
-        <v>155</v>
-      </c>
-      <c r="C51" s="53" t="s">
+    <row r="52" spans="1:3" ht="38.25">
+      <c r="A52" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" s="46" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B52" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="C52" s="53" t="s">
+    <row r="53" spans="1:3" ht="76.5">
+      <c r="A53" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" s="47" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B53" s="54" t="s">
+      <c r="C53" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="C53" s="53" t="s">
+    </row>
+    <row r="54" spans="1:3" ht="76.5">
+      <c r="A54" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" s="46" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B54" s="54" t="s">
-        <v>163</v>
-      </c>
-      <c r="C54" s="53" t="s">
+    <row r="55" spans="1:3" ht="63.75">
+      <c r="A55" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="46" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B55" s="54" t="s">
-        <v>163</v>
-      </c>
-      <c r="C55" s="53" t="s">
+    <row r="56" spans="1:3" ht="153">
+      <c r="A56" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" s="47" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B56" s="54" t="s">
+      <c r="C56" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="C56" s="53" t="s">
+    </row>
+    <row r="57" spans="1:3" ht="242.25">
+      <c r="A57" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" s="47" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="242.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B57" s="54" t="s">
+      <c r="C57" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="C57" s="53" t="s">
+    </row>
+    <row r="58" spans="1:3" ht="38.25">
+      <c r="A58" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B58" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="46" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B58" s="54" t="s">
-        <v>169</v>
-      </c>
-      <c r="C58" s="53" t="s">
+    <row r="59" spans="1:3" ht="76.5">
+      <c r="A59" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B59" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" s="46" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B59" s="54" t="s">
-        <v>169</v>
-      </c>
-      <c r="C59" s="53" t="s">
+    <row r="60" spans="1:3" ht="25.5">
+      <c r="A60" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B60" s="47" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B60" s="54" t="s">
+      <c r="C60" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="C60" s="53" t="s">
+    </row>
+    <row r="61" spans="1:3" ht="38.25">
+      <c r="A61" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B61" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="C61" s="46" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="51" x14ac:dyDescent="0.25">
-      <c r="A61" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B61" s="54" t="s">
-        <v>173</v>
-      </c>
-      <c r="C61" s="53" t="s">
+    <row r="62" spans="1:3" ht="25.5">
+      <c r="A62" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B62" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="C62" s="46" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B62" s="54" t="s">
-        <v>173</v>
-      </c>
-      <c r="C62" s="53" t="s">
+    <row r="63" spans="1:3" ht="51">
+      <c r="A63" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B63" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="C63" s="46" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="51" x14ac:dyDescent="0.25">
-      <c r="A63" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B63" s="54" t="s">
-        <v>173</v>
-      </c>
-      <c r="C63" s="53" t="s">
+    <row r="64" spans="1:3" ht="63.75">
+      <c r="A64" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B64" s="47" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B64" s="54" t="s">
+      <c r="C64" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="C64" s="53" t="s">
+    </row>
+    <row r="65" spans="1:3" ht="76.5">
+      <c r="A65" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B65" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="46" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B65" s="54" t="s">
-        <v>178</v>
-      </c>
-      <c r="C65" s="53" t="s">
+    <row r="66" spans="1:3" ht="76.5">
+      <c r="A66" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B66" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C66" s="46" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B66" s="54" t="s">
-        <v>178</v>
-      </c>
-      <c r="C66" s="53" t="s">
+    <row r="67" spans="1:3" ht="89.25">
+      <c r="A67" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C67" s="46" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B67" s="54" t="s">
-        <v>178</v>
-      </c>
-      <c r="C67" s="53" t="s">
+    <row r="68" spans="1:3" ht="63.75">
+      <c r="A68" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B68" s="47" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B68" s="54" t="s">
+      <c r="C68" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="C68" s="53" t="s">
+    </row>
+    <row r="69" spans="1:3" ht="38.25">
+      <c r="A69" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B69" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="C69" s="46" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B69" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="C69" s="53" t="s">
+    <row r="70" spans="1:3" ht="38.25">
+      <c r="A70" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="C70" s="46" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B70" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="C70" s="53" t="s">
+    <row r="71" spans="1:3" ht="51">
+      <c r="A71" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B71" s="47" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="51" x14ac:dyDescent="0.25">
-      <c r="A71" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B71" s="54" t="s">
+      <c r="C71" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="C71" s="53" t="s">
+    </row>
+    <row r="72" spans="1:3" ht="76.5">
+      <c r="A72" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C72" s="46" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B72" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="C72" s="53" t="s">
+    <row r="73" spans="1:3" ht="63.75">
+      <c r="A73" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C73" s="46" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B73" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="C73" s="53" t="s">
+    <row r="74" spans="1:3" ht="89.25">
+      <c r="A74" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C74" s="46" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B74" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="C74" s="53" t="s">
+    <row r="75" spans="1:3" ht="25.5">
+      <c r="A75" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" s="46" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B75" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="C75" s="53" t="s">
+    <row r="76" spans="1:3" ht="38.25">
+      <c r="A76" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C76" s="46" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B76" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="C76" s="53" t="s">
+    <row r="77" spans="1:3" ht="89.25">
+      <c r="A77" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C77" s="46" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B77" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="C77" s="53" t="s">
+    <row r="78" spans="1:3" ht="89.25">
+      <c r="A78" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B78" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C78" s="46" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B78" s="54" t="s">
-        <v>187</v>
-      </c>
-      <c r="C78" s="53" t="s">
+    <row r="79" spans="1:3" ht="127.5">
+      <c r="A79" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B79" s="47" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B79" s="54" t="s">
+      <c r="C79" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="C79" s="53" t="s">
+    </row>
+    <row r="80" spans="1:3" ht="140.25">
+      <c r="A80" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="C80" s="46" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B80" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="C80" s="53" t="s">
+    <row r="81" spans="1:3" ht="38.25">
+      <c r="A81" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B81" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" s="46" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B81" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="C81" s="53" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>